<commit_message>
add sort and filter by color examples
</commit_message>
<xml_diff>
--- a/CS/SpreadsheetDocServerAPIPart2/Document.xlsx
+++ b/CS/SpreadsheetDocServerAPIPart2/Document.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4EFF95-19A8-444F-99B3-46610C3CCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D29DD6B-C22A-45DE-9DE8-B6C22F49408E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4448" yWindow="3458" windowWidth="13447" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,13 @@
     <sheet name="FormatTable" sheetId="9" state="hidden" r:id="rId5"/>
     <sheet name="Custom Table Style" sheetId="10" state="hidden" r:id="rId6"/>
     <sheet name="Duplicate Table Style" sheetId="11" state="hidden" r:id="rId7"/>
-    <sheet name="SortSample" sheetId="20" state="hidden" r:id="rId8"/>
+    <sheet name="SortSample" sheetId="20" r:id="rId8"/>
     <sheet name="Grouping" sheetId="22" state="hidden" r:id="rId9"/>
     <sheet name="Grouping and Outline" sheetId="23" state="hidden" r:id="rId10"/>
     <sheet name="Regional Sales" sheetId="25" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">SortSample!$A$2:$F$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">SortSample!$B$2:$B$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -352,7 +353,7 @@
     <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(_)"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,8 +518,67 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFCC00"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -639,6 +699,54 @@
         <fgColor rgb="FFE6F9F9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -682,7 +790,7 @@
     <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyFont="0"/>
     <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyFont="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,24 +808,22 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -752,13 +858,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="21" fillId="17" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -776,7 +882,20 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -822,6 +941,11 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Custom Style" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -905,6 +1029,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC00"/>
       <color rgb="FFF5DEB3"/>
       <color rgb="FF66FF33"/>
     </mruColors>
@@ -1286,7 +1411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
@@ -1311,11 +1436,6 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B2" s="5" t="s">
@@ -1610,326 +1730,327 @@
   <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="31.3984375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="15.86328125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="31.3984375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.86328125" style="15" customWidth="1"/>
     <col min="5" max="5" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="48">
         <v>6750</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="20">
         <v>42018</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="49">
         <v>8200</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>44727</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="48">
         <v>7500</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="20">
         <v>44698</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="47">
         <v>4500</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="20">
         <v>42024</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="48">
         <v>9100</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="20">
         <v>42081</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="50">
         <v>13500</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="20">
         <v>42226</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="47">
         <v>3550</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="20">
         <v>42043</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="47">
         <v>1250</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="47">
         <v>2100</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="20">
         <v>42082</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="47">
         <v>4250</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="20">
         <v>42146</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="48">
         <v>5200</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="20">
         <v>42169</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="47">
         <v>3800</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="20">
         <v>42108</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="48">
         <v>5500</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="50">
         <v>12500</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="20">
         <v>42262</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="48">
         <v>6500</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="20">
         <v>41743</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="48">
         <v>6250</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="20">
         <v>41653</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="50">
         <v>11800</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="20">
         <v>41804</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="48">
         <v>8600</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="20">
         <v>41743</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="48">
         <v>5325</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="20">
         <v>41653</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21">
+      <c r="C22" s="19"/>
+      <c r="D22" s="49">
         <v>9600</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="20">
         <v>41804</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="48">
         <v>6580</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="20">
         <v>41743</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1953,662 +2074,662 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43" t="s">
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="43"/>
-      <c r="L3" s="36" t="s">
+      <c r="K3" s="54"/>
+      <c r="L3" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="N3" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="24">
+      <c r="B4" s="22">
         <f ca="1">NOW()-14</f>
-        <v>44566.842758449071</v>
-      </c>
-      <c r="C4" s="25">
+        <v>45408.645012499997</v>
+      </c>
+      <c r="C4" s="23">
         <v>212340</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45">
+      <c r="E4" s="55"/>
+      <c r="F4" s="56">
         <v>250</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="26">
+      <c r="G4" s="56"/>
+      <c r="H4" s="24">
         <v>130</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="25">
         <v>12.42</v>
       </c>
-      <c r="J4" s="46">
+      <c r="J4" s="57">
         <v>50</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="27">
+      <c r="K4" s="57"/>
+      <c r="L4" s="25">
         <v>8</v>
       </c>
-      <c r="M4" s="27">
+      <c r="M4" s="25">
         <v>19.3</v>
       </c>
-      <c r="N4" s="40">
+      <c r="N4" s="38">
         <f t="shared" ref="N4:N18" si="0">SUM(F4:M4)</f>
         <v>469.72</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <f ca="1">NOW()-13</f>
-        <v>44567.842758449071</v>
-      </c>
-      <c r="C5" s="29">
+        <v>45409.645012499997</v>
+      </c>
+      <c r="C5" s="27">
         <v>289043</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48">
+      <c r="E5" s="58"/>
+      <c r="F5" s="59">
         <v>250</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="30">
+      <c r="G5" s="59"/>
+      <c r="H5" s="28">
         <v>0</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="29">
         <v>26.6</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="60">
         <v>45</v>
       </c>
-      <c r="K5" s="49"/>
-      <c r="L5" s="31">
+      <c r="K5" s="60"/>
+      <c r="L5" s="29">
         <v>7.8</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="29">
         <v>29.3</v>
       </c>
-      <c r="N5" s="41">
+      <c r="N5" s="39">
         <f t="shared" si="0"/>
         <v>358.70000000000005</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="24">
+      <c r="B6" s="22">
         <f ca="1">NOW()-12</f>
-        <v>44568.842758449071</v>
-      </c>
-      <c r="C6" s="25">
+        <v>45410.645012499997</v>
+      </c>
+      <c r="C6" s="23">
         <v>212340</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51">
+      <c r="E6" s="61"/>
+      <c r="F6" s="62">
         <v>0</v>
       </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="26">
+      <c r="G6" s="62"/>
+      <c r="H6" s="24">
         <v>10</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="25">
         <v>0</v>
       </c>
-      <c r="J6" s="52">
+      <c r="J6" s="63">
         <v>58</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="27">
+      <c r="K6" s="63"/>
+      <c r="L6" s="25">
         <v>2.79</v>
       </c>
-      <c r="M6" s="27">
+      <c r="M6" s="25">
         <v>12.3</v>
       </c>
-      <c r="N6" s="40">
+      <c r="N6" s="38">
         <f t="shared" si="0"/>
         <v>83.09</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="28">
+      <c r="B7" s="26">
         <f ca="1">NOW()-11</f>
-        <v>44569.842758449071</v>
-      </c>
-      <c r="C7" s="29">
+        <v>45411.645012499997</v>
+      </c>
+      <c r="C7" s="27">
         <v>216049</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="48">
+      <c r="E7" s="58"/>
+      <c r="F7" s="59">
         <v>0</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="30">
+      <c r="G7" s="59"/>
+      <c r="H7" s="28">
         <v>30</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="29">
         <v>0</v>
       </c>
-      <c r="J7" s="49">
+      <c r="J7" s="60">
         <v>60</v>
       </c>
-      <c r="K7" s="49"/>
-      <c r="L7" s="31">
+      <c r="K7" s="60"/>
+      <c r="L7" s="29">
         <v>9.7899999999999991</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="29">
         <v>122.3</v>
       </c>
-      <c r="N7" s="41">
+      <c r="N7" s="39">
         <f t="shared" si="0"/>
         <v>222.08999999999997</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="24">
+      <c r="B8" s="22">
         <f ca="1">NOW()-10</f>
-        <v>44570.842758449071</v>
-      </c>
-      <c r="C8" s="25">
+        <v>45412.645012499997</v>
+      </c>
+      <c r="C8" s="23">
         <v>292352</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51">
+      <c r="E8" s="61"/>
+      <c r="F8" s="62">
         <v>295.5</v>
       </c>
-      <c r="G8" s="51"/>
-      <c r="H8" s="26">
+      <c r="G8" s="62"/>
+      <c r="H8" s="24">
         <v>150</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="25">
         <v>10.48</v>
       </c>
-      <c r="J8" s="52">
+      <c r="J8" s="63">
         <v>45</v>
       </c>
-      <c r="K8" s="52"/>
-      <c r="L8" s="27">
+      <c r="K8" s="63"/>
+      <c r="L8" s="25">
         <v>9.32</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="25">
         <v>59</v>
       </c>
-      <c r="N8" s="40">
+      <c r="N8" s="38">
         <f t="shared" si="0"/>
         <v>569.29999999999995</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="28">
+      <c r="B9" s="26">
         <f ca="1">NOW()-9</f>
-        <v>44571.842758449071</v>
-      </c>
-      <c r="C9" s="29">
+        <v>45413.645012499997</v>
+      </c>
+      <c r="C9" s="27">
         <v>567384</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48">
+      <c r="E9" s="58"/>
+      <c r="F9" s="59">
         <v>295.5</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="30">
+      <c r="G9" s="59"/>
+      <c r="H9" s="28">
         <v>30</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="29">
         <v>20.37</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="60">
         <v>50</v>
       </c>
-      <c r="K9" s="49"/>
-      <c r="L9" s="31">
+      <c r="K9" s="60"/>
+      <c r="L9" s="29">
         <v>9.1199999999999992</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="29">
         <v>30.07</v>
       </c>
-      <c r="N9" s="41">
+      <c r="N9" s="39">
         <f t="shared" si="0"/>
         <v>435.06</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="24">
+      <c r="B10" s="22">
         <f ca="1">NOW()-8</f>
-        <v>44572.842758449071</v>
-      </c>
-      <c r="C10" s="25">
+        <v>45414.645012499997</v>
+      </c>
+      <c r="C10" s="23">
         <v>890733</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="51">
+      <c r="E10" s="61"/>
+      <c r="F10" s="62">
         <v>349</v>
       </c>
-      <c r="G10" s="51"/>
-      <c r="H10" s="26">
+      <c r="G10" s="62"/>
+      <c r="H10" s="24">
         <v>70</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="25">
         <v>15.07</v>
       </c>
-      <c r="J10" s="52">
+      <c r="J10" s="63">
         <v>45</v>
       </c>
-      <c r="K10" s="52"/>
-      <c r="L10" s="27">
+      <c r="K10" s="63"/>
+      <c r="L10" s="25">
         <v>14.05</v>
       </c>
-      <c r="M10" s="27">
+      <c r="M10" s="25">
         <v>100.93</v>
       </c>
-      <c r="N10" s="40">
+      <c r="N10" s="38">
         <f t="shared" si="0"/>
         <v>594.04999999999995</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="28">
+      <c r="B11" s="26">
         <f ca="1">NOW()-7</f>
-        <v>44573.842758449071</v>
-      </c>
-      <c r="C11" s="29">
+        <v>45415.645012499997</v>
+      </c>
+      <c r="C11" s="27">
         <v>578292</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48">
+      <c r="E11" s="58"/>
+      <c r="F11" s="59">
         <v>349</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="30">
+      <c r="G11" s="59"/>
+      <c r="H11" s="28">
         <v>0</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="29">
         <v>6.8</v>
       </c>
-      <c r="J11" s="49">
+      <c r="J11" s="60">
         <v>60</v>
       </c>
-      <c r="K11" s="49"/>
-      <c r="L11" s="31">
+      <c r="K11" s="60"/>
+      <c r="L11" s="29">
         <v>3.7</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="29">
         <v>302.8</v>
       </c>
-      <c r="N11" s="41">
+      <c r="N11" s="39">
         <f t="shared" si="0"/>
         <v>722.3</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="24">
+      <c r="B12" s="22">
         <f ca="1">NOW()-6</f>
-        <v>44574.842758449071</v>
-      </c>
-      <c r="C12" s="25">
+        <v>45416.645012499997</v>
+      </c>
+      <c r="C12" s="23">
         <v>199123</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51">
+      <c r="E12" s="61"/>
+      <c r="F12" s="62">
         <v>349</v>
       </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="26">
+      <c r="G12" s="62"/>
+      <c r="H12" s="24">
         <v>90</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="25">
         <v>13.6</v>
       </c>
-      <c r="J12" s="52">
+      <c r="J12" s="63">
         <v>50</v>
       </c>
-      <c r="K12" s="52"/>
-      <c r="L12" s="27">
+      <c r="K12" s="63"/>
+      <c r="L12" s="25">
         <v>2.6</v>
       </c>
-      <c r="M12" s="27">
+      <c r="M12" s="25">
         <v>23</v>
       </c>
-      <c r="N12" s="40">
+      <c r="N12" s="38">
         <f t="shared" si="0"/>
         <v>528.20000000000005</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="28">
+      <c r="B13" s="26">
         <f ca="1">NOW()-5</f>
-        <v>44575.842758449071</v>
-      </c>
-      <c r="C13" s="29">
+        <v>45417.645012499997</v>
+      </c>
+      <c r="C13" s="27">
         <v>423509</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="48">
+      <c r="E13" s="58"/>
+      <c r="F13" s="59">
         <v>0</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="30">
+      <c r="G13" s="59"/>
+      <c r="H13" s="28">
         <v>0</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="29">
         <v>37.5</v>
       </c>
-      <c r="J13" s="49">
+      <c r="J13" s="60">
         <v>60</v>
       </c>
-      <c r="K13" s="49"/>
-      <c r="L13" s="31">
+      <c r="K13" s="60"/>
+      <c r="L13" s="29">
         <v>2.04</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="29">
         <v>20</v>
       </c>
-      <c r="N13" s="41">
+      <c r="N13" s="39">
         <f t="shared" si="0"/>
         <v>119.54</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="24">
+      <c r="B14" s="22">
         <f ca="1">NOW()-4</f>
-        <v>44576.842758449071</v>
-      </c>
-      <c r="C14" s="25">
+        <v>45418.645012499997</v>
+      </c>
+      <c r="C14" s="23">
         <v>543288</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="51">
+      <c r="E14" s="61"/>
+      <c r="F14" s="62">
         <v>0</v>
       </c>
-      <c r="G14" s="51"/>
-      <c r="H14" s="26">
+      <c r="G14" s="62"/>
+      <c r="H14" s="24">
         <v>90</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="25">
         <v>14.2</v>
       </c>
-      <c r="J14" s="52">
+      <c r="J14" s="63">
         <v>70</v>
       </c>
-      <c r="K14" s="52"/>
-      <c r="L14" s="27">
+      <c r="K14" s="63"/>
+      <c r="L14" s="25">
         <v>0.2</v>
       </c>
-      <c r="M14" s="27">
+      <c r="M14" s="25">
         <v>12</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14" s="38">
         <f t="shared" si="0"/>
         <v>186.39999999999998</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="28">
+      <c r="B15" s="26">
         <f ca="1">NOW()-3</f>
-        <v>44577.842758449071</v>
-      </c>
-      <c r="C15" s="29">
+        <v>45419.645012499997</v>
+      </c>
+      <c r="C15" s="27">
         <v>457382</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48">
+      <c r="E15" s="58"/>
+      <c r="F15" s="59">
         <v>205</v>
       </c>
-      <c r="G15" s="48"/>
-      <c r="H15" s="30">
+      <c r="G15" s="59"/>
+      <c r="H15" s="28">
         <v>125</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="29">
         <v>16</v>
       </c>
-      <c r="J15" s="49">
+      <c r="J15" s="60">
         <v>45</v>
       </c>
-      <c r="K15" s="49"/>
-      <c r="L15" s="31">
+      <c r="K15" s="60"/>
+      <c r="L15" s="29">
         <v>14</v>
       </c>
-      <c r="M15" s="31">
+      <c r="M15" s="29">
         <v>35.39</v>
       </c>
-      <c r="N15" s="41">
+      <c r="N15" s="39">
         <f t="shared" si="0"/>
         <v>440.39</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="24">
+      <c r="B16" s="22">
         <f ca="1">NOW()-2</f>
-        <v>44578.842758449071</v>
-      </c>
-      <c r="C16" s="25">
+        <v>45420.645012499997</v>
+      </c>
+      <c r="C16" s="23">
         <v>584839</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51">
+      <c r="E16" s="61"/>
+      <c r="F16" s="62">
         <v>205</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="26">
+      <c r="G16" s="62"/>
+      <c r="H16" s="24">
         <v>0</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="25">
         <v>10.029999999999999</v>
       </c>
-      <c r="J16" s="52">
+      <c r="J16" s="63">
         <v>40</v>
       </c>
-      <c r="K16" s="52"/>
-      <c r="L16" s="27">
+      <c r="K16" s="63"/>
+      <c r="L16" s="25">
         <v>12.01</v>
       </c>
-      <c r="M16" s="27">
+      <c r="M16" s="25">
         <v>30</v>
       </c>
-      <c r="N16" s="40">
+      <c r="N16" s="38">
         <f t="shared" si="0"/>
         <v>297.04000000000002</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="28">
+      <c r="B17" s="26">
         <f ca="1">NOW()-1</f>
-        <v>44579.842758449071</v>
-      </c>
-      <c r="C17" s="29">
+        <v>45421.645012499997</v>
+      </c>
+      <c r="C17" s="27">
         <v>483922</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48">
+      <c r="E17" s="58"/>
+      <c r="F17" s="59">
         <v>205</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="30">
+      <c r="G17" s="59"/>
+      <c r="H17" s="28">
         <v>0</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="29">
         <v>26</v>
       </c>
-      <c r="J17" s="49">
+      <c r="J17" s="60">
         <v>55</v>
       </c>
-      <c r="K17" s="49"/>
-      <c r="L17" s="31">
+      <c r="K17" s="60"/>
+      <c r="L17" s="29">
         <v>9.1999999999999993</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M17" s="29">
         <v>60</v>
       </c>
-      <c r="N17" s="41">
+      <c r="N17" s="39">
         <f t="shared" si="0"/>
         <v>355.2</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="24">
+      <c r="B18" s="22">
         <f ca="1">NOW()</f>
-        <v>44580.842758449071</v>
-      </c>
-      <c r="C18" s="25">
+        <v>45422.645012499997</v>
+      </c>
+      <c r="C18" s="23">
         <v>890763</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51">
+      <c r="E18" s="61"/>
+      <c r="F18" s="62">
         <v>205</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="26">
+      <c r="G18" s="62"/>
+      <c r="H18" s="24">
         <v>125</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="25">
         <v>9.5</v>
       </c>
-      <c r="J18" s="52">
+      <c r="J18" s="63">
         <v>45</v>
       </c>
-      <c r="K18" s="52"/>
-      <c r="L18" s="27">
+      <c r="K18" s="63"/>
+      <c r="L18" s="25">
         <v>1.03</v>
       </c>
-      <c r="M18" s="27">
+      <c r="M18" s="25">
         <v>143</v>
       </c>
-      <c r="N18" s="40">
+      <c r="N18" s="38">
         <f t="shared" si="0"/>
         <v>528.53</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="54">
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65">
         <f>SUM(F4:G18)</f>
         <v>2958</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="38">
+      <c r="G19" s="65"/>
+      <c r="H19" s="36">
         <f t="shared" ref="H19:I19" si="1">SUM(H3:H18)</f>
         <v>850</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="36">
         <f t="shared" si="1"/>
         <v>218.56999999999996</v>
       </c>
-      <c r="J19" s="54">
+      <c r="J19" s="65">
         <f>SUM(J4:K18)</f>
         <v>778</v>
       </c>
-      <c r="K19" s="54"/>
-      <c r="L19" s="38">
+      <c r="K19" s="65"/>
+      <c r="L19" s="36">
         <f t="shared" ref="L19:M19" si="2">SUM(L4:L18)</f>
         <v>105.65000000000002</v>
       </c>
-      <c r="M19" s="38">
+      <c r="M19" s="36">
         <f t="shared" si="2"/>
         <v>999.39</v>
       </c>
-      <c r="N19" s="33"/>
+      <c r="N19" s="31"/>
     </row>
     <row r="20" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="42" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="N20" s="39">
+      <c r="N20" s="37">
         <f>SUM(N4:N18)</f>
         <v>5909.61</v>
       </c>
@@ -2685,48 +2806,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3040,13 +3161,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
@@ -3132,13 +3253,13 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
@@ -3244,8 +3365,8 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3258,397 +3379,397 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>142958</v>
+      </c>
+      <c r="E3">
+        <v>1524915</v>
+      </c>
+      <c r="F3" s="70">
+        <v>1707540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>34017</v>
+      </c>
+      <c r="E4">
+        <v>1577040</v>
+      </c>
+      <c r="F4" s="71">
+        <v>997061</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5">
+        <v>310384</v>
+      </c>
+      <c r="E5">
+        <v>14419400</v>
+      </c>
+      <c r="F5" s="71">
+        <v>962909</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>1348932</v>
+      </c>
+      <c r="E6">
+        <v>5949786</v>
+      </c>
+      <c r="F6" s="71">
+        <v>956207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <v>194946</v>
+      </c>
+      <c r="E7">
+        <v>2143035</v>
+      </c>
+      <c r="F7" s="71">
+        <v>854740</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8">
+        <v>22268</v>
+      </c>
+      <c r="E8">
+        <v>1138262</v>
+      </c>
+      <c r="F8" s="71">
+        <v>774122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9">
+        <v>1224614</v>
+      </c>
+      <c r="E9">
+        <v>1710917</v>
+      </c>
+      <c r="F9" s="72">
+        <v>328726</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3">
+      <c r="D10">
         <v>40412</v>
       </c>
-      <c r="E3">
+      <c r="E10">
         <v>368736</v>
       </c>
-      <c r="F3">
+      <c r="F10" s="72">
         <v>278040</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4">
-        <v>22268</v>
-      </c>
-      <c r="E4">
-        <v>1138262</v>
-      </c>
-      <c r="F4">
-        <v>774122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5">
-        <v>194946</v>
-      </c>
-      <c r="E5">
-        <v>2143035</v>
-      </c>
-      <c r="F5">
-        <v>854740</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>27448</v>
+      </c>
+      <c r="E11">
+        <v>526811</v>
+      </c>
+      <c r="F11" s="72">
+        <v>214969</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6">
-        <v>34017</v>
-      </c>
-      <c r="E6">
-        <v>1577040</v>
-      </c>
-      <c r="F6">
-        <v>997061</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12">
+        <v>113423</v>
+      </c>
+      <c r="E12">
+        <v>1034941</v>
+      </c>
+      <c r="F12" s="72">
+        <v>195820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7">
-        <v>1348932</v>
-      </c>
-      <c r="E7">
-        <v>5949786</v>
-      </c>
-      <c r="F7">
-        <v>956207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13">
+        <v>239871</v>
+      </c>
+      <c r="E13">
+        <v>709266</v>
+      </c>
+      <c r="F13" s="72">
+        <v>190457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14">
+        <v>50133</v>
+      </c>
+      <c r="E14">
+        <v>363241</v>
+      </c>
+      <c r="F14" s="72">
+        <v>122104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15">
+        <v>72752</v>
+      </c>
+      <c r="E15">
+        <v>731144</v>
+      </c>
+      <c r="F15" s="73">
+        <v>77482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D8">
+      <c r="D16">
         <v>62787</v>
       </c>
-      <c r="E8">
+      <c r="E16">
         <v>2548315</v>
       </c>
-      <c r="F8">
+      <c r="F16" s="73">
         <v>55150</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17">
+        <v>46077</v>
+      </c>
+      <c r="E17">
+        <v>1380109</v>
+      </c>
+      <c r="F17" s="73">
+        <v>50599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18">
+        <v>126536</v>
+      </c>
+      <c r="E18">
+        <v>5495379</v>
+      </c>
+      <c r="F18" s="73">
+        <v>37780</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D9">
+      <c r="D19">
         <v>82302</v>
       </c>
-      <c r="E9">
+      <c r="E19">
         <v>3284474</v>
       </c>
-      <c r="F9">
+      <c r="F19" s="73">
         <v>35703</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10">
-        <v>1224614</v>
-      </c>
-      <c r="E10">
-        <v>1710917</v>
-      </c>
-      <c r="F10">
-        <v>328726</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11">
-        <v>239871</v>
-      </c>
-      <c r="E11">
-        <v>709266</v>
-      </c>
-      <c r="F11">
-        <v>190457</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B20" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D12">
+      <c r="D20">
         <v>60551</v>
       </c>
-      <c r="E12">
+      <c r="E20">
         <v>2041955</v>
       </c>
-      <c r="F12">
+      <c r="F20" s="73">
         <v>30134</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13">
-        <v>126536</v>
-      </c>
-      <c r="E13">
-        <v>5495379</v>
-      </c>
-      <c r="F13">
-        <v>37780</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14">
-        <v>113423</v>
-      </c>
-      <c r="E14">
-        <v>1034941</v>
-      </c>
-      <c r="F14">
-        <v>195820</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15">
-        <v>142958</v>
-      </c>
-      <c r="E15">
-        <v>1524915</v>
-      </c>
-      <c r="F15">
-        <v>1707540</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16">
-        <v>27448</v>
-      </c>
-      <c r="E16">
-        <v>526811</v>
-      </c>
-      <c r="F16">
-        <v>214969</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17">
-        <v>50133</v>
-      </c>
-      <c r="E17">
-        <v>363241</v>
-      </c>
-      <c r="F17">
-        <v>122104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18">
-        <v>48184</v>
-      </c>
-      <c r="E18">
-        <v>1014890</v>
-      </c>
-      <c r="F18">
-        <v>9926</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19">
-        <v>46077</v>
-      </c>
-      <c r="E19">
-        <v>1380109</v>
-      </c>
-      <c r="F19">
-        <v>50599</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20">
-        <v>72752</v>
-      </c>
-      <c r="E20">
-        <v>731144</v>
-      </c>
-      <c r="F20">
-        <v>77482</v>
-      </c>
-    </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="A21" s="45" t="s">
         <v>53</v>
       </c>
       <c r="B21" t="s">
@@ -3663,28 +3784,28 @@
       <c r="E21">
         <v>2548315</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="74">
         <v>24291</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>47</v>
+      <c r="A22" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D22">
-        <v>310384</v>
+        <v>48184</v>
       </c>
       <c r="E22">
-        <v>14419400</v>
-      </c>
-      <c r="F22">
-        <v>962909</v>
+        <v>1014890</v>
+      </c>
+      <c r="F22" s="74">
+        <v>9926</v>
       </c>
     </row>
   </sheetData>
@@ -3711,11 +3832,6 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="5" t="s">

</xml_diff>